<commit_message>
corrección de diseño de documento
</commit_message>
<xml_diff>
--- a/Entregables/III. Planeación del Proyecto TI/III.6 Estimacion de Costos/APPMO-SP_ECO_v1.0.xlsx
+++ b/Entregables/III. Planeación del Proyecto TI/III.6 Estimacion de Costos/APPMO-SP_ECO_v1.0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FRANC\Desktop\APPMO-SP\Entregables\Estimacion de Costos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FRANC\Desktop\SM-ROOT\Entregables\III. Planeación del Proyecto TI\III.6 Estimacion de Costos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1367,7 +1367,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -1377,11 +1377,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1488,8 +1486,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1501,35 +1497,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1557,9 +1529,6 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1569,6 +1538,27 @@
     <xf numFmtId="164" fontId="5" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1608,15 +1598,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -1626,17 +1607,53 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1920,10 +1937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Y50"/>
+  <dimension ref="A1:Y50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="S40" sqref="S40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1952,1397 +1969,1397 @@
   <sheetData>
     <row r="1" spans="2:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:25" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="79" t="s">
+      <c r="C2" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="80"/>
-      <c r="E2" s="85" t="s">
+      <c r="D2" s="74"/>
+      <c r="E2" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="85" t="s">
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="87"/>
-      <c r="O2" s="85" t="s">
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="86"/>
-      <c r="Q2" s="86"/>
-      <c r="R2" s="86"/>
-      <c r="S2" s="87"/>
-      <c r="T2" s="83" t="s">
+      <c r="P2" s="80"/>
+      <c r="Q2" s="80"/>
+      <c r="R2" s="80"/>
+      <c r="S2" s="81"/>
+      <c r="T2" s="77" t="s">
         <v>8</v>
       </c>
       <c r="W2" s="3"/>
     </row>
     <row r="3" spans="2:25" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="78"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="30" t="s">
+      <c r="B3" s="72"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="F3" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="48" t="s">
+      <c r="G3" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="48" t="s">
+      <c r="H3" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="49" t="s">
+      <c r="I3" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="47" t="s">
+      <c r="J3" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="48" t="s">
+      <c r="K3" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="48" t="s">
+      <c r="L3" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="48" t="s">
+      <c r="M3" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="49" t="s">
+      <c r="N3" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="47" t="s">
+      <c r="O3" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="48" t="s">
+      <c r="P3" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="48" t="s">
+      <c r="Q3" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="48" t="s">
+      <c r="R3" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="S3" s="49" t="s">
+      <c r="S3" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="T3" s="84"/>
+      <c r="T3" s="78"/>
       <c r="W3" s="3"/>
     </row>
     <row r="4" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="95" t="s">
+      <c r="B4" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="96" t="s">
+      <c r="C4" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="97"/>
-      <c r="E4" s="22" t="s">
+      <c r="D4" s="68"/>
+      <c r="E4" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="6">
         <v>8</v>
       </c>
-      <c r="H4" s="24">
+      <c r="H4" s="22">
         <v>108.92</v>
       </c>
-      <c r="I4" s="26">
+      <c r="I4" s="24">
         <f>H4*G4</f>
         <v>871.36</v>
       </c>
-      <c r="J4" s="29" t="s">
+      <c r="J4" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="K4" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="L4" s="29">
+      <c r="L4" s="27">
         <v>10</v>
       </c>
-      <c r="M4" s="32">
+      <c r="M4" s="30">
         <v>2</v>
       </c>
-      <c r="N4" s="33">
+      <c r="N4" s="31">
         <f>M4*L4</f>
         <v>20</v>
       </c>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="42"/>
-      <c r="T4" s="43">
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="40"/>
+      <c r="T4" s="41">
         <f>SUM(I4,N4,S4)</f>
         <v>891.36</v>
       </c>
       <c r="Y4" s="3"/>
     </row>
     <row r="5" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="94"/>
-      <c r="C5" s="88" t="s">
+      <c r="B5" s="65"/>
+      <c r="C5" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="89"/>
-      <c r="E5" s="15" t="s">
+      <c r="D5" s="63"/>
+      <c r="E5" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G5" s="4">
         <v>12</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="17">
         <v>108.92</v>
       </c>
-      <c r="I5" s="27">
+      <c r="I5" s="25">
         <f t="shared" ref="I5:I34" si="0">H5*G5</f>
         <v>1307.04</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="K5" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="L5" s="17">
+      <c r="L5" s="15">
         <v>5</v>
       </c>
-      <c r="M5" s="20">
+      <c r="M5" s="18">
         <v>2</v>
       </c>
-      <c r="N5" s="34">
+      <c r="N5" s="32">
         <f>M5*L5</f>
         <v>10</v>
       </c>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="38"/>
-      <c r="T5" s="37">
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="36"/>
+      <c r="T5" s="35">
         <f t="shared" ref="T5:T34" si="1">SUM(I5,N5,S5)</f>
         <v>1317.04</v>
       </c>
       <c r="Y5" s="3"/>
     </row>
     <row r="6" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="94"/>
-      <c r="C6" s="88" t="s">
+      <c r="B6" s="65"/>
+      <c r="C6" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="89"/>
-      <c r="E6" s="15" t="s">
+      <c r="D6" s="63"/>
+      <c r="E6" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G6" s="4">
         <v>8</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="17">
         <v>108.92</v>
       </c>
-      <c r="I6" s="27">
+      <c r="I6" s="25">
         <f t="shared" si="0"/>
         <v>871.36</v>
       </c>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="20"/>
-      <c r="S6" s="38"/>
-      <c r="T6" s="37">
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="36"/>
+      <c r="T6" s="35">
         <f t="shared" si="1"/>
         <v>871.36</v>
       </c>
       <c r="Y6" s="3"/>
     </row>
     <row r="7" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="94"/>
-      <c r="C7" s="88" t="s">
+      <c r="B7" s="65"/>
+      <c r="C7" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="89"/>
-      <c r="E7" s="15" t="s">
+      <c r="D7" s="63"/>
+      <c r="E7" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G7" s="4">
         <v>8</v>
       </c>
-      <c r="H7" s="20">
+      <c r="H7" s="18">
         <v>53.48</v>
       </c>
-      <c r="I7" s="27">
+      <c r="I7" s="25">
         <f t="shared" si="0"/>
         <v>427.84</v>
       </c>
-      <c r="J7" s="17" t="s">
+      <c r="J7" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="L7" s="17">
+      <c r="L7" s="15">
         <v>10</v>
       </c>
-      <c r="M7" s="20">
+      <c r="M7" s="18">
         <v>2</v>
       </c>
-      <c r="N7" s="34">
+      <c r="N7" s="32">
         <f>M7*L7</f>
         <v>20</v>
       </c>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="20"/>
-      <c r="S7" s="38"/>
-      <c r="T7" s="37">
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="36"/>
+      <c r="T7" s="35">
         <f t="shared" si="1"/>
         <v>447.84</v>
       </c>
     </row>
     <row r="8" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="94"/>
-      <c r="C8" s="88" t="s">
+      <c r="B8" s="65"/>
+      <c r="C8" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="89"/>
-      <c r="E8" s="15" t="s">
+      <c r="D8" s="63"/>
+      <c r="E8" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G8" s="4">
         <v>12</v>
       </c>
-      <c r="H8" s="20">
+      <c r="H8" s="18">
         <v>53.48</v>
       </c>
-      <c r="I8" s="27">
+      <c r="I8" s="25">
         <f t="shared" si="0"/>
         <v>641.76</v>
       </c>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="20"/>
-      <c r="S8" s="38"/>
-      <c r="T8" s="37">
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="32"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="36"/>
+      <c r="T8" s="35">
         <f t="shared" si="1"/>
         <v>641.76</v>
       </c>
     </row>
     <row r="9" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="94"/>
-      <c r="C9" s="88" t="s">
+      <c r="B9" s="65"/>
+      <c r="C9" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="89"/>
-      <c r="E9" s="15" t="s">
+      <c r="D9" s="63"/>
+      <c r="E9" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G9" s="4">
         <v>12</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="17">
         <v>108.92</v>
       </c>
-      <c r="I9" s="27">
+      <c r="I9" s="25">
         <f t="shared" si="0"/>
         <v>1307.04</v>
       </c>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="20"/>
-      <c r="S9" s="38"/>
-      <c r="T9" s="37">
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="18"/>
+      <c r="S9" s="36"/>
+      <c r="T9" s="35">
         <f t="shared" si="1"/>
         <v>1307.04</v>
       </c>
     </row>
     <row r="10" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="94"/>
-      <c r="C10" s="88" t="s">
+      <c r="B10" s="65"/>
+      <c r="C10" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="89"/>
-      <c r="E10" s="15" t="s">
+      <c r="D10" s="63"/>
+      <c r="E10" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G10" s="4">
         <v>16</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="18">
         <v>33.94</v>
       </c>
-      <c r="I10" s="27">
+      <c r="I10" s="25">
         <f t="shared" si="0"/>
         <v>543.04</v>
       </c>
-      <c r="J10" s="17" t="s">
+      <c r="J10" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="K10" s="17" t="s">
+      <c r="K10" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="L10" s="17">
+      <c r="L10" s="15">
         <v>5</v>
       </c>
-      <c r="M10" s="20">
+      <c r="M10" s="18">
         <v>2</v>
       </c>
-      <c r="N10" s="34">
+      <c r="N10" s="32">
         <f>M10*L10</f>
         <v>10</v>
       </c>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="20"/>
-      <c r="S10" s="38"/>
-      <c r="T10" s="37">
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="36"/>
+      <c r="T10" s="35">
         <f t="shared" si="1"/>
         <v>553.04</v>
       </c>
     </row>
     <row r="11" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="94"/>
-      <c r="C11" s="88" t="s">
+      <c r="B11" s="65"/>
+      <c r="C11" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="89"/>
-      <c r="E11" s="15" t="s">
+      <c r="D11" s="63"/>
+      <c r="E11" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G11" s="4">
         <v>44</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="18">
         <v>53.48</v>
       </c>
-      <c r="I11" s="27">
+      <c r="I11" s="25">
         <f t="shared" si="0"/>
         <v>2353.12</v>
       </c>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="20"/>
-      <c r="S11" s="38"/>
-      <c r="T11" s="37">
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="18"/>
+      <c r="S11" s="36"/>
+      <c r="T11" s="35">
         <f t="shared" si="1"/>
         <v>2353.12</v>
       </c>
     </row>
     <row r="12" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="94"/>
-      <c r="C12" s="88" t="s">
+      <c r="B12" s="65"/>
+      <c r="C12" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="89"/>
-      <c r="E12" s="15" t="s">
+      <c r="D12" s="63"/>
+      <c r="E12" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G12" s="4">
         <v>24</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="17">
         <v>108.92</v>
       </c>
-      <c r="I12" s="27">
+      <c r="I12" s="25">
         <f t="shared" si="0"/>
         <v>2614.08</v>
       </c>
-      <c r="J12" s="17" t="s">
+      <c r="J12" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="K12" s="17" t="s">
+      <c r="K12" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="L12" s="17">
+      <c r="L12" s="15">
         <v>10</v>
       </c>
-      <c r="M12" s="20">
+      <c r="M12" s="18">
         <v>2</v>
       </c>
-      <c r="N12" s="34">
+      <c r="N12" s="32">
         <f>M12*L12</f>
         <v>20</v>
       </c>
-      <c r="O12" s="17"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="17"/>
-      <c r="R12" s="20"/>
-      <c r="S12" s="38"/>
-      <c r="T12" s="37">
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="18"/>
+      <c r="S12" s="36"/>
+      <c r="T12" s="35">
         <f t="shared" si="1"/>
         <v>2634.08</v>
       </c>
     </row>
     <row r="13" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="94" t="s">
+      <c r="B13" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="88" t="s">
+      <c r="C13" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="89"/>
-      <c r="E13" s="15" t="s">
+      <c r="D13" s="63"/>
+      <c r="E13" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G13" s="4">
         <v>24</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="17">
         <v>108.92</v>
       </c>
-      <c r="I13" s="27">
+      <c r="I13" s="25">
         <f t="shared" si="0"/>
         <v>2614.08</v>
       </c>
-      <c r="J13" s="17" t="s">
+      <c r="J13" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="K13" s="17" t="s">
+      <c r="K13" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="L13" s="17">
+      <c r="L13" s="15">
         <v>10</v>
       </c>
-      <c r="M13" s="20">
+      <c r="M13" s="18">
         <v>2</v>
       </c>
-      <c r="N13" s="34">
+      <c r="N13" s="32">
         <f>M13*L13</f>
         <v>20</v>
       </c>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="20"/>
-      <c r="S13" s="38"/>
-      <c r="T13" s="37">
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="18"/>
+      <c r="S13" s="36"/>
+      <c r="T13" s="35">
         <f t="shared" si="1"/>
         <v>2634.08</v>
       </c>
     </row>
     <row r="14" spans="2:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="94"/>
-      <c r="C14" s="88" t="s">
+      <c r="B14" s="65"/>
+      <c r="C14" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="89"/>
-      <c r="E14" s="15" t="s">
+      <c r="D14" s="63"/>
+      <c r="E14" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G14" s="4">
         <v>12</v>
       </c>
-      <c r="H14" s="20">
+      <c r="H14" s="18">
         <v>33.94</v>
       </c>
-      <c r="I14" s="27">
+      <c r="I14" s="25">
         <f t="shared" si="0"/>
         <v>407.28</v>
       </c>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="34"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="20"/>
-      <c r="S14" s="38"/>
-      <c r="T14" s="37">
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="32"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="36"/>
+      <c r="T14" s="35">
         <f t="shared" si="1"/>
         <v>407.28</v>
       </c>
     </row>
     <row r="15" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="94"/>
-      <c r="C15" s="88" t="s">
+      <c r="B15" s="65"/>
+      <c r="C15" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="89"/>
-      <c r="E15" s="15" t="s">
+      <c r="D15" s="63"/>
+      <c r="E15" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G15" s="4">
         <v>16</v>
       </c>
-      <c r="H15" s="20">
+      <c r="H15" s="18">
         <v>33.94</v>
       </c>
-      <c r="I15" s="27">
+      <c r="I15" s="25">
         <f t="shared" si="0"/>
         <v>543.04</v>
       </c>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="34"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="20"/>
-      <c r="S15" s="38"/>
-      <c r="T15" s="37">
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="32"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="36"/>
+      <c r="T15" s="35">
         <f t="shared" si="1"/>
         <v>543.04</v>
       </c>
     </row>
     <row r="16" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="94"/>
-      <c r="C16" s="88" t="s">
+      <c r="B16" s="65"/>
+      <c r="C16" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="89"/>
-      <c r="E16" s="15" t="s">
+      <c r="D16" s="63"/>
+      <c r="E16" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G16" s="4">
         <v>8</v>
       </c>
-      <c r="H16" s="19">
+      <c r="H16" s="17">
         <v>108.92</v>
       </c>
-      <c r="I16" s="27">
+      <c r="I16" s="25">
         <f t="shared" si="0"/>
         <v>871.36</v>
       </c>
-      <c r="J16" s="17" t="s">
+      <c r="J16" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="K16" s="17" t="s">
+      <c r="K16" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="L16" s="17">
+      <c r="L16" s="15">
         <v>10</v>
       </c>
-      <c r="M16" s="20">
+      <c r="M16" s="18">
         <v>2</v>
       </c>
-      <c r="N16" s="34">
+      <c r="N16" s="32">
         <f>M16*L16</f>
         <v>20</v>
       </c>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="20"/>
-      <c r="S16" s="38"/>
-      <c r="T16" s="37">
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="18"/>
+      <c r="S16" s="36"/>
+      <c r="T16" s="35">
         <f t="shared" si="1"/>
         <v>891.36</v>
       </c>
     </row>
     <row r="17" spans="2:20" ht="15" x14ac:dyDescent="0.3">
-      <c r="B17" s="94" t="s">
+      <c r="B17" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="88" t="s">
+      <c r="C17" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G17" s="4">
         <v>28</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H17" s="17">
         <v>108.92</v>
       </c>
-      <c r="I17" s="27">
+      <c r="I17" s="25">
         <f t="shared" si="0"/>
         <v>3049.76</v>
       </c>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="34"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="20"/>
-      <c r="S17" s="38"/>
-      <c r="T17" s="37">
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="18"/>
+      <c r="S17" s="36"/>
+      <c r="T17" s="35">
         <f t="shared" si="1"/>
         <v>3049.76</v>
       </c>
     </row>
     <row r="18" spans="2:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="94"/>
-      <c r="C18" s="88"/>
-      <c r="D18" s="13" t="s">
+      <c r="B18" s="65"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G18" s="4">
         <v>24</v>
       </c>
-      <c r="H18" s="20">
+      <c r="H18" s="18">
         <v>33.94</v>
       </c>
-      <c r="I18" s="27">
+      <c r="I18" s="25">
         <f t="shared" si="0"/>
         <v>814.56</v>
       </c>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="34"/>
-      <c r="O18" s="17" t="s">
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="P18" s="17" t="s">
+      <c r="P18" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="Q18" s="17">
+      <c r="Q18" s="15">
         <v>1</v>
       </c>
-      <c r="R18" s="66">
+      <c r="R18" s="54">
         <v>300</v>
       </c>
-      <c r="S18" s="67">
+      <c r="S18" s="55">
         <f>R18*Q18</f>
         <v>300</v>
       </c>
-      <c r="T18" s="37">
+      <c r="T18" s="35">
         <f t="shared" si="1"/>
         <v>1114.56</v>
       </c>
     </row>
     <row r="19" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="94"/>
-      <c r="C19" s="88" t="s">
+      <c r="B19" s="65"/>
+      <c r="C19" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G19" s="4">
         <v>32</v>
       </c>
-      <c r="H19" s="20">
+      <c r="H19" s="18">
         <v>97.51</v>
       </c>
-      <c r="I19" s="27">
+      <c r="I19" s="25">
         <f t="shared" si="0"/>
         <v>3120.32</v>
       </c>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="34"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="17"/>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="20"/>
-      <c r="S19" s="38"/>
-      <c r="T19" s="37">
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="18"/>
+      <c r="S19" s="36"/>
+      <c r="T19" s="35">
         <f t="shared" si="1"/>
         <v>3120.32</v>
       </c>
     </row>
     <row r="20" spans="2:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="94"/>
-      <c r="C20" s="88"/>
-      <c r="D20" s="13" t="s">
+      <c r="B20" s="65"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G20" s="4">
         <v>32</v>
       </c>
-      <c r="H20" s="20">
+      <c r="H20" s="18">
         <v>97.51</v>
       </c>
-      <c r="I20" s="27">
+      <c r="I20" s="25">
         <f t="shared" si="0"/>
         <v>3120.32</v>
       </c>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="17"/>
-      <c r="P20" s="17"/>
-      <c r="Q20" s="17"/>
-      <c r="R20" s="20"/>
-      <c r="S20" s="38"/>
-      <c r="T20" s="37">
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="32"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="36"/>
+      <c r="T20" s="35">
         <f t="shared" si="1"/>
         <v>3120.32</v>
       </c>
     </row>
     <row r="21" spans="2:20" ht="15" x14ac:dyDescent="0.3">
-      <c r="B21" s="94"/>
-      <c r="C21" s="88"/>
-      <c r="D21" s="13" t="s">
+      <c r="B21" s="65"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G21" s="4">
         <v>40</v>
       </c>
-      <c r="H21" s="20">
+      <c r="H21" s="18">
         <v>97.51</v>
       </c>
-      <c r="I21" s="27">
+      <c r="I21" s="25">
         <f t="shared" si="0"/>
         <v>3900.4</v>
       </c>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="34"/>
-      <c r="O21" s="17"/>
-      <c r="P21" s="17"/>
-      <c r="Q21" s="17"/>
-      <c r="R21" s="20"/>
-      <c r="S21" s="38"/>
-      <c r="T21" s="37">
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="32"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="36"/>
+      <c r="T21" s="35">
         <f t="shared" si="1"/>
         <v>3900.4</v>
       </c>
     </row>
     <row r="22" spans="2:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="94"/>
-      <c r="C22" s="88"/>
-      <c r="D22" s="13" t="s">
+      <c r="B22" s="65"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G22" s="4">
         <v>32</v>
       </c>
-      <c r="H22" s="20">
+      <c r="H22" s="18">
         <v>97.51</v>
       </c>
-      <c r="I22" s="27">
+      <c r="I22" s="25">
         <f t="shared" si="0"/>
         <v>3120.32</v>
       </c>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="34"/>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17"/>
-      <c r="Q22" s="17"/>
-      <c r="R22" s="20"/>
-      <c r="S22" s="38"/>
-      <c r="T22" s="37">
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="32"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="18"/>
+      <c r="S22" s="36"/>
+      <c r="T22" s="35">
         <f t="shared" si="1"/>
         <v>3120.32</v>
       </c>
     </row>
     <row r="23" spans="2:20" ht="15" x14ac:dyDescent="0.3">
-      <c r="B23" s="94"/>
-      <c r="C23" s="88"/>
-      <c r="D23" s="13" t="s">
+      <c r="B23" s="65"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G23" s="4">
         <v>40</v>
       </c>
-      <c r="H23" s="20">
+      <c r="H23" s="18">
         <v>97.51</v>
       </c>
-      <c r="I23" s="27">
+      <c r="I23" s="25">
         <f t="shared" si="0"/>
         <v>3900.4</v>
       </c>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="34"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="20"/>
-      <c r="S23" s="38"/>
-      <c r="T23" s="37">
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="32"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="36"/>
+      <c r="T23" s="35">
         <f t="shared" si="1"/>
         <v>3900.4</v>
       </c>
     </row>
     <row r="24" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="94"/>
-      <c r="C24" s="88" t="s">
+      <c r="B24" s="65"/>
+      <c r="C24" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E24" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G24" s="4">
         <v>28</v>
       </c>
-      <c r="H24" s="20">
+      <c r="H24" s="18">
         <v>53.48</v>
       </c>
-      <c r="I24" s="27">
+      <c r="I24" s="25">
         <f t="shared" si="0"/>
         <v>1497.4399999999998</v>
       </c>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="34"/>
-      <c r="O24" s="40"/>
-      <c r="P24" s="17"/>
-      <c r="Q24" s="17"/>
-      <c r="R24" s="20"/>
-      <c r="S24" s="38"/>
-      <c r="T24" s="37">
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="38"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="36"/>
+      <c r="T24" s="35">
         <f t="shared" si="1"/>
         <v>1497.4399999999998</v>
       </c>
     </row>
     <row r="25" spans="2:20" ht="15" x14ac:dyDescent="0.3">
-      <c r="B25" s="94"/>
-      <c r="C25" s="88"/>
-      <c r="D25" s="13" t="s">
+      <c r="B25" s="65"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="E25" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G25" s="4">
         <v>20</v>
       </c>
-      <c r="H25" s="20">
+      <c r="H25" s="18">
         <v>53.48</v>
       </c>
-      <c r="I25" s="27">
+      <c r="I25" s="25">
         <f t="shared" si="0"/>
         <v>1069.5999999999999</v>
       </c>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="34"/>
-      <c r="O25" s="17"/>
-      <c r="P25" s="17"/>
-      <c r="Q25" s="17"/>
-      <c r="R25" s="20" t="s">
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="S25" s="38"/>
-      <c r="T25" s="37">
+      <c r="S25" s="36"/>
+      <c r="T25" s="35">
         <f t="shared" si="1"/>
         <v>1069.5999999999999</v>
       </c>
     </row>
     <row r="26" spans="2:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="94"/>
-      <c r="C26" s="88"/>
-      <c r="D26" s="13" t="s">
+      <c r="B26" s="65"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="15" t="s">
+      <c r="E26" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G26" s="4">
         <v>32</v>
       </c>
-      <c r="H26" s="20">
+      <c r="H26" s="18">
         <v>53.48</v>
       </c>
-      <c r="I26" s="27">
+      <c r="I26" s="25">
         <f>H26*G26</f>
         <v>1711.36</v>
       </c>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="34"/>
-      <c r="O26" s="17"/>
-      <c r="P26" s="17"/>
-      <c r="Q26" s="17"/>
-      <c r="R26" s="20"/>
-      <c r="S26" s="38"/>
-      <c r="T26" s="37">
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="36"/>
+      <c r="T26" s="35">
         <f t="shared" si="1"/>
         <v>1711.36</v>
       </c>
     </row>
     <row r="27" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="94"/>
-      <c r="C27" s="11" t="s">
+      <c r="B27" s="65"/>
+      <c r="C27" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G27" s="4">
         <v>20</v>
       </c>
-      <c r="H27" s="20">
+      <c r="H27" s="18">
         <v>97.51</v>
       </c>
-      <c r="I27" s="27">
+      <c r="I27" s="25">
         <f t="shared" si="0"/>
         <v>1950.2</v>
       </c>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="34"/>
-      <c r="O27" s="17"/>
-      <c r="P27" s="17"/>
-      <c r="Q27" s="17"/>
-      <c r="R27" s="20"/>
-      <c r="S27" s="38"/>
-      <c r="T27" s="37">
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="15"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="15"/>
+      <c r="R27" s="18"/>
+      <c r="S27" s="36"/>
+      <c r="T27" s="35">
         <f>SUM(I27,N27,S27)</f>
         <v>1950.2</v>
       </c>
     </row>
     <row r="28" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="90" t="s">
+      <c r="B28" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="88" t="s">
+      <c r="C28" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="89"/>
-      <c r="E28" s="15" t="s">
+      <c r="D28" s="63"/>
+      <c r="E28" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G28" s="4">
         <v>64</v>
       </c>
-      <c r="H28" s="19">
+      <c r="H28" s="17">
         <v>108.92</v>
       </c>
-      <c r="I28" s="27">
+      <c r="I28" s="25">
         <f t="shared" si="0"/>
         <v>6970.88</v>
       </c>
-      <c r="J28" s="17" t="s">
+      <c r="J28" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="K28" s="17" t="s">
+      <c r="K28" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="L28" s="17">
+      <c r="L28" s="15">
         <v>15</v>
       </c>
-      <c r="M28" s="20">
+      <c r="M28" s="18">
         <v>2</v>
       </c>
-      <c r="N28" s="34">
+      <c r="N28" s="32">
         <f>M28*L28</f>
         <v>30</v>
       </c>
-      <c r="O28" s="17"/>
-      <c r="P28" s="17"/>
-      <c r="Q28" s="17"/>
-      <c r="R28" s="20"/>
-      <c r="S28" s="38"/>
-      <c r="T28" s="37">
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="18"/>
+      <c r="S28" s="36"/>
+      <c r="T28" s="35">
         <f t="shared" si="1"/>
         <v>7000.88</v>
       </c>
     </row>
     <row r="29" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="90"/>
-      <c r="C29" s="88" t="s">
+      <c r="B29" s="64"/>
+      <c r="C29" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="89"/>
-      <c r="E29" s="15" t="s">
+      <c r="D29" s="63"/>
+      <c r="E29" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G29" s="4">
         <v>12</v>
       </c>
-      <c r="H29" s="19">
+      <c r="H29" s="17">
         <v>108.92</v>
       </c>
-      <c r="I29" s="27">
+      <c r="I29" s="25">
         <f t="shared" si="0"/>
         <v>1307.04</v>
       </c>
-      <c r="J29" s="17"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="34"/>
-      <c r="O29" s="17"/>
-      <c r="P29" s="17"/>
-      <c r="Q29" s="17"/>
-      <c r="R29" s="20"/>
-      <c r="S29" s="38"/>
-      <c r="T29" s="37">
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="32"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="15"/>
+      <c r="R29" s="18"/>
+      <c r="S29" s="36"/>
+      <c r="T29" s="35">
         <f t="shared" si="1"/>
         <v>1307.04</v>
       </c>
     </row>
     <row r="30" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="88" t="s">
+      <c r="C30" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="89"/>
-      <c r="E30" s="15" t="s">
+      <c r="D30" s="63"/>
+      <c r="E30" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="F30" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G30" s="4">
         <v>80</v>
       </c>
-      <c r="H30" s="20">
+      <c r="H30" s="18">
         <v>33.94</v>
       </c>
-      <c r="I30" s="27">
+      <c r="I30" s="25">
         <f t="shared" si="0"/>
         <v>2715.2</v>
       </c>
-      <c r="J30" s="17" t="s">
+      <c r="J30" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="K30" s="17" t="s">
+      <c r="K30" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="L30" s="17">
+      <c r="L30" s="15">
         <v>25</v>
       </c>
-      <c r="M30" s="20">
+      <c r="M30" s="18">
         <v>2</v>
       </c>
-      <c r="N30" s="34">
+      <c r="N30" s="32">
         <f>M30*L30</f>
         <v>50</v>
       </c>
-      <c r="O30" s="17"/>
-      <c r="P30" s="17"/>
-      <c r="Q30" s="17"/>
-      <c r="R30" s="20"/>
-      <c r="S30" s="38"/>
-      <c r="T30" s="37">
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="18"/>
+      <c r="S30" s="36"/>
+      <c r="T30" s="35">
         <f t="shared" si="1"/>
         <v>2765.2</v>
       </c>
     </row>
     <row r="31" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="90" t="s">
+      <c r="B31" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="88" t="s">
+      <c r="C31" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="D31" s="89"/>
-      <c r="E31" s="15" t="s">
+      <c r="D31" s="63"/>
+      <c r="E31" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F31" s="10" t="s">
+      <c r="F31" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G31" s="4">
         <v>16</v>
       </c>
-      <c r="H31" s="19">
+      <c r="H31" s="17">
         <v>108.92</v>
       </c>
-      <c r="I31" s="27">
+      <c r="I31" s="25">
         <f t="shared" si="0"/>
         <v>1742.72</v>
       </c>
-      <c r="J31" s="17" t="s">
+      <c r="J31" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="K31" s="17" t="s">
+      <c r="K31" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="L31" s="17">
+      <c r="L31" s="15">
         <v>5</v>
       </c>
-      <c r="M31" s="20">
+      <c r="M31" s="18">
         <v>2</v>
       </c>
-      <c r="N31" s="34">
+      <c r="N31" s="32">
         <f>M31*L31</f>
         <v>10</v>
       </c>
-      <c r="O31" s="17"/>
-      <c r="P31" s="17"/>
-      <c r="Q31" s="17"/>
-      <c r="R31" s="20"/>
-      <c r="S31" s="38"/>
-      <c r="T31" s="37">
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="18"/>
+      <c r="S31" s="36"/>
+      <c r="T31" s="35">
         <f t="shared" si="1"/>
         <v>1752.72</v>
       </c>
     </row>
     <row r="32" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="90"/>
-      <c r="C32" s="88" t="s">
+      <c r="B32" s="64"/>
+      <c r="C32" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="D32" s="89"/>
-      <c r="E32" s="15" t="s">
+      <c r="D32" s="63"/>
+      <c r="E32" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="F32" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G32" s="4">
         <v>28</v>
       </c>
-      <c r="H32" s="20">
+      <c r="H32" s="18">
         <v>33.94</v>
       </c>
-      <c r="I32" s="27">
+      <c r="I32" s="25">
         <f t="shared" si="0"/>
         <v>950.31999999999994</v>
       </c>
-      <c r="J32" s="17" t="s">
+      <c r="J32" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="K32" s="17" t="s">
+      <c r="K32" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="L32" s="17">
+      <c r="L32" s="15">
         <v>40</v>
       </c>
-      <c r="M32" s="20">
+      <c r="M32" s="18">
         <v>2</v>
       </c>
-      <c r="N32" s="34">
+      <c r="N32" s="32">
         <f>M32*L32</f>
         <v>80</v>
       </c>
-      <c r="O32" s="17"/>
-      <c r="P32" s="17"/>
-      <c r="Q32" s="17"/>
-      <c r="R32" s="20"/>
-      <c r="S32" s="38"/>
-      <c r="T32" s="37">
+      <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15"/>
+      <c r="R32" s="18"/>
+      <c r="S32" s="36"/>
+      <c r="T32" s="35">
         <f t="shared" si="1"/>
         <v>1030.32</v>
       </c>
     </row>
-    <row r="33" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="90"/>
-      <c r="C33" s="88" t="s">
+    <row r="33" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="64"/>
+      <c r="C33" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="D33" s="89"/>
-      <c r="E33" s="15" t="s">
+      <c r="D33" s="63"/>
+      <c r="E33" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F33" s="10" t="s">
+      <c r="F33" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G33" s="4">
         <v>28</v>
       </c>
-      <c r="H33" s="20">
+      <c r="H33" s="18">
         <v>53.48</v>
       </c>
-      <c r="I33" s="27">
+      <c r="I33" s="25">
         <f t="shared" si="0"/>
         <v>1497.4399999999998</v>
       </c>
-      <c r="J33" s="17"/>
-      <c r="K33" s="17"/>
-      <c r="L33" s="17"/>
-      <c r="M33" s="20"/>
-      <c r="N33" s="35"/>
-      <c r="O33" s="17"/>
-      <c r="P33" s="17"/>
-      <c r="Q33" s="17"/>
-      <c r="R33" s="20"/>
-      <c r="S33" s="38"/>
-      <c r="T33" s="37">
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="33"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="18"/>
+      <c r="S33" s="36"/>
+      <c r="T33" s="35">
         <f t="shared" si="1"/>
         <v>1497.4399999999998</v>
       </c>
     </row>
-    <row r="34" spans="2:20" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="91"/>
-      <c r="C34" s="92" t="s">
+    <row r="34" spans="1:20" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="82"/>
+      <c r="C34" s="83" t="s">
         <v>53</v>
       </c>
-      <c r="D34" s="93"/>
-      <c r="E34" s="9" t="s">
+      <c r="D34" s="84"/>
+      <c r="E34" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F34" s="14" t="s">
+      <c r="F34" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="G34" s="6">
+      <c r="G34" s="5">
         <v>16</v>
       </c>
-      <c r="H34" s="25">
+      <c r="H34" s="23">
         <v>108.92</v>
       </c>
-      <c r="I34" s="28">
+      <c r="I34" s="26">
         <f t="shared" si="0"/>
         <v>1742.72</v>
       </c>
-      <c r="J34" s="18"/>
-      <c r="K34" s="18"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="21"/>
-      <c r="N34" s="36"/>
-      <c r="O34" s="18"/>
-      <c r="P34" s="18"/>
-      <c r="Q34" s="18"/>
-      <c r="R34" s="21"/>
-      <c r="S34" s="39"/>
-      <c r="T34" s="41">
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="34"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="16"/>
+      <c r="R34" s="19"/>
+      <c r="S34" s="37"/>
+      <c r="T34" s="39">
         <f t="shared" si="1"/>
         <v>1742.72</v>
       </c>
     </row>
-    <row r="35" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="46"/>
+    <row r="35" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="42"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -3358,235 +3375,274 @@
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
-      <c r="R35" s="75" t="s">
+      <c r="R35" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="S35" s="76"/>
-      <c r="T35" s="50">
+      <c r="S35" s="70"/>
+      <c r="T35" s="46">
         <f>SUM(T4:T34)</f>
         <v>60143.400000000009</v>
       </c>
     </row>
-    <row r="36" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="37" spans="2:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="44" t="s">
+    <row r="36" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="86" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="45" t="s">
+      <c r="C37" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="E37" s="51" t="s">
+      <c r="D37" s="85"/>
+      <c r="E37" s="88" t="s">
         <v>72</v>
       </c>
-      <c r="F37" s="52"/>
-    </row>
-    <row r="38" spans="2:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="7" t="s">
+      <c r="F37" s="89"/>
+      <c r="G37" s="85"/>
+      <c r="H37" s="85"/>
+      <c r="I37" s="85"/>
+      <c r="J37" s="85"/>
+    </row>
+    <row r="38" spans="1:20" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="90" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="90" t="s">
         <v>66</v>
       </c>
-      <c r="E38" s="53">
+      <c r="D38" s="85"/>
+      <c r="E38" s="91">
         <v>1</v>
       </c>
-      <c r="F38" s="70">
+      <c r="F38" s="92">
         <f>-$T$35</f>
         <v>-60143.400000000009</v>
       </c>
-      <c r="H38" s="54" t="s">
+      <c r="G38" s="85"/>
+      <c r="H38" s="93" t="s">
         <v>73</v>
       </c>
-      <c r="I38" s="55" t="s">
+      <c r="I38" s="94" t="s">
         <v>74</v>
       </c>
-      <c r="J38" s="56" t="s">
+      <c r="J38" s="95" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="2:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="5" t="s">
+    <row r="39" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="3"/>
+      <c r="B39" s="96" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="E39" s="53">
+      <c r="D39" s="85"/>
+      <c r="E39" s="91">
         <v>2</v>
       </c>
-      <c r="F39" s="70">
+      <c r="F39" s="92">
         <f t="shared" ref="F39:F45" si="2">$I$44</f>
         <v>31000</v>
       </c>
-      <c r="H39" s="57" t="s">
+      <c r="G39" s="85"/>
+      <c r="H39" s="97" t="s">
         <v>76</v>
       </c>
-      <c r="I39" s="71">
+      <c r="I39" s="98">
         <v>5000</v>
       </c>
-      <c r="J39" s="60" t="s">
+      <c r="J39" s="99" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="2:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="5" t="s">
+    <row r="40" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="96" t="s">
         <v>55</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="96" t="s">
         <v>68</v>
       </c>
-      <c r="E40" s="53">
+      <c r="D40" s="85"/>
+      <c r="E40" s="91">
         <v>3</v>
       </c>
-      <c r="F40" s="70">
+      <c r="F40" s="92">
         <f t="shared" si="2"/>
         <v>31000</v>
       </c>
-      <c r="H40" s="57" t="s">
+      <c r="G40" s="85"/>
+      <c r="H40" s="97" t="s">
         <v>78</v>
       </c>
-      <c r="I40" s="71">
+      <c r="I40" s="98">
         <v>8000</v>
       </c>
-      <c r="J40" s="59" t="s">
+      <c r="J40" s="100" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="2:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="5" t="s">
+    <row r="41" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="96" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="96" t="s">
         <v>69</v>
       </c>
-      <c r="E41" s="53">
+      <c r="D41" s="85"/>
+      <c r="E41" s="91">
         <v>4</v>
       </c>
-      <c r="F41" s="70">
+      <c r="F41" s="92">
         <f t="shared" si="2"/>
         <v>31000</v>
       </c>
-      <c r="H41" s="57" t="s">
+      <c r="G41" s="85"/>
+      <c r="H41" s="97" t="s">
         <v>79</v>
       </c>
-      <c r="I41" s="71">
+      <c r="I41" s="98">
         <v>5000</v>
       </c>
-      <c r="J41" s="59" t="s">
+      <c r="J41" s="100" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="2:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="5" t="s">
+    <row r="42" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="96" t="s">
         <v>70</v>
       </c>
-      <c r="E42" s="53">
+      <c r="D42" s="85"/>
+      <c r="E42" s="91">
         <v>5</v>
       </c>
-      <c r="F42" s="70">
+      <c r="F42" s="92">
         <f t="shared" si="2"/>
         <v>31000</v>
       </c>
-      <c r="H42" s="57" t="s">
+      <c r="G42" s="85"/>
+      <c r="H42" s="97" t="s">
         <v>80</v>
       </c>
-      <c r="I42" s="71">
+      <c r="I42" s="98">
         <v>5000</v>
       </c>
-      <c r="J42" s="59" t="s">
+      <c r="J42" s="100" t="s">
         <v>81</v>
       </c>
-      <c r="L42" s="63"/>
-    </row>
-    <row r="43" spans="2:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E43" s="53">
+      <c r="L42" s="51"/>
+    </row>
+    <row r="43" spans="1:20" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="85"/>
+      <c r="C43" s="85"/>
+      <c r="D43" s="85"/>
+      <c r="E43" s="91">
         <v>6</v>
       </c>
-      <c r="F43" s="70">
+      <c r="F43" s="92">
         <f t="shared" si="2"/>
         <v>31000</v>
       </c>
-      <c r="H43" s="57" t="s">
+      <c r="G43" s="85"/>
+      <c r="H43" s="97" t="s">
         <v>82</v>
       </c>
-      <c r="I43" s="71">
+      <c r="I43" s="98">
         <v>8000</v>
       </c>
-      <c r="J43" s="59" t="s">
+      <c r="J43" s="100" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="2:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E44" s="53">
+    <row r="44" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E44" s="47">
         <v>7</v>
       </c>
-      <c r="F44" s="70">
+      <c r="F44" s="58">
         <f t="shared" si="2"/>
         <v>31000</v>
       </c>
-      <c r="H44" s="58" t="s">
+      <c r="H44" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="I44" s="72">
+      <c r="I44" s="59">
         <f>SUM(I39:I43)</f>
         <v>31000</v>
       </c>
       <c r="J44" s="1"/>
     </row>
-    <row r="45" spans="2:20" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E45" s="53">
+    <row r="45" spans="1:20" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E45" s="47">
         <v>8</v>
       </c>
-      <c r="F45" s="70">
+      <c r="F45" s="58">
         <f t="shared" si="2"/>
         <v>31000</v>
       </c>
     </row>
-    <row r="46" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="47" spans="2:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E47" s="61" t="s">
+    <row r="46" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="47" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E47" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="F47" s="74">
+      <c r="F47" s="61">
         <f>NPV(30%,F39:F45)</f>
         <v>86865.480661479203</v>
       </c>
-      <c r="K47" s="63"/>
-    </row>
-    <row r="48" spans="2:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E48" s="62" t="s">
+      <c r="K47" s="51"/>
+    </row>
+    <row r="48" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E48" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="F48" s="69">
+      <c r="F48" s="57">
         <f>IRR(F38:F45)</f>
         <v>0.4827185989002718</v>
       </c>
-      <c r="G48" s="68"/>
-      <c r="H48" s="68"/>
+      <c r="G48" s="56"/>
+      <c r="H48" s="56"/>
     </row>
     <row r="49" spans="5:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E49" s="64" t="s">
+      <c r="E49" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="F49" s="73">
+      <c r="F49" s="60">
         <f>T35</f>
         <v>60143.400000000009</v>
       </c>
     </row>
     <row r="50" spans="5:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E50" s="64" t="s">
+      <c r="E50" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="F50" s="65">
+      <c r="F50" s="53">
         <f>F47/F49</f>
         <v>1.4443061193992888</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:N2"/>
+    <mergeCell ref="O2:S2"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C23"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="R35:S35"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D3"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="B17:B27"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
@@ -3603,25 +3659,6 @@
     <mergeCell ref="B4:B12"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="R35:S35"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:N2"/>
-    <mergeCell ref="O2:S2"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="B17:B27"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>